<commit_message>
Update excel in saucedemo-e2e-framework
</commit_message>
<xml_diff>
--- a/primers-and-refreshers/saucedemo-e2e-framework/src/test/resources/valid_logins.xlsx
+++ b/primers-and-refreshers/saucedemo-e2e-framework/src/test/resources/valid_logins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BachTran\Desktop\211018-jwa-extended\training-workspaces\testng-workspace\saucedemo-e2e-framework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BachTran\Desktop\211018-jwa-extended\training\primers-and-refreshers\saucedemo-e2e-framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06113008-2E1C-4E88-9E7C-0490F9AE7278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B139F78-217E-4156-B0CC-74B25BE2779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26535" yWindow="2970" windowWidth="18900" windowHeight="10470" xr2:uid="{4A9D5417-B290-47DA-84FE-5158BDA55A02}"/>
+    <workbookView xWindow="-21015" yWindow="2700" windowWidth="18900" windowHeight="10470" xr2:uid="{4A9D5417-B290-47DA-84FE-5158BDA55A02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>standard_user</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>dslajflksdjfsldkf</t>
-  </si>
-  <si>
-    <t>sdfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -403,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC912EB-45C1-4891-A7C1-DCE202315320}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,14 +433,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>